<commit_message>
Data changes as of 11/16/2018
Data changes as of 11/16/2018 includes the .xlsx files. Only "Test Cases.xlsx" was changed. These enable the tests to run in TESTING and STAGING environments.
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases Laa.xlsx
+++ b/src/com/data/Test Cases Laa.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12450" windowHeight="6690" tabRatio="157" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13725" tabRatio="157" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="84">
   <si>
     <t>TCID</t>
   </si>
@@ -249,6 +249,24 @@
   </si>
   <si>
     <t>Construction Code Determination Form (CCD1)</t>
+  </si>
+  <si>
+    <t>Subsequent On Antenna</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>Antenna ::  :: I ::  :: approved ::  ::  ::  :: rome18 ::  ::  :: exempted</t>
+  </si>
+  <si>
+    <t>LaatOnAntenna</t>
+  </si>
+  <si>
+    <t>owner_info</t>
+  </si>
+  <si>
+    <t>APPLEROME18@GMAIL.COM</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1021,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1081,6 +1099,9 @@
     </xf>
     <xf numFmtId="49" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="212">
@@ -1302,6 +1323,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1597,7 +1621,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="12.75"/>
@@ -1794,7 +1818,9 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="27"/>
+      <c r="A23" s="27" t="s">
+        <v>81</v>
+      </c>
       <c r="C23" s="24" t="s">
         <v>3</v>
       </c>
@@ -1849,169 +1875,170 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N78"/>
+  <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showFormulas="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F66" sqref="F66"/>
+      <selection pane="topRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="35.28515625" defaultRowHeight="29.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="35.28515625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" style="8" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="2" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="35.28515625" style="8"/>
-    <col min="15" max="16384" width="35.28515625" style="9"/>
+    <col min="1" max="1" width="14.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="13" customWidth="1"/>
+    <col min="3" max="4" width="35.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="9" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="8" customWidth="1"/>
+    <col min="12" max="12" width="2" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="35.28515625" style="8"/>
+    <col min="16" max="16384" width="35.28515625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="18" customFormat="1" ht="29.25" customHeight="1">
+    <row r="1" spans="1:15" s="18" customFormat="1" ht="12.75" customHeight="1">
       <c r="A1" s="15"/>
       <c r="B1" s="16"/>
       <c r="C1" s="17"/>
-      <c r="D1" s="15"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
-      <c r="J1" s="17"/>
+      <c r="J1" s="15"/>
       <c r="K1" s="17"/>
       <c r="L1" s="17"/>
       <c r="M1" s="17"/>
       <c r="N1" s="17"/>
-    </row>
-    <row r="2" spans="1:14" ht="12.75">
-      <c r="A2" s="21"/>
-    </row>
-    <row r="3" spans="1:14" s="18" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-    </row>
-    <row r="4" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="O1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A2" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+    </row>
+    <row r="4" spans="1:15" ht="12.75" customHeight="1">
+      <c r="A4" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="12.75" customHeight="1">
+      <c r="A5" s="21"/>
+    </row>
+    <row r="6" spans="1:15" ht="12.75" customHeight="1">
+      <c r="A6" s="21"/>
+    </row>
+    <row r="7" spans="1:15" s="18" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+    </row>
+    <row r="8" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A8" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-    </row>
-    <row r="5" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A5" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-    </row>
-    <row r="6" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A6" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-    </row>
-    <row r="7" spans="1:14" ht="12.75">
-      <c r="A7" s="21"/>
-    </row>
-    <row r="8" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A8" s="27" t="s">
-        <v>54</v>
-      </c>
       <c r="B8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="I8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
-    </row>
-    <row r="9" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A9" s="11" t="s">
         <v>2</v>
       </c>
@@ -2022,81 +2049,91 @@
         <v>7</v>
       </c>
       <c r="D9" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="F9" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="G9" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="H9" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="I9" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="29" t="s">
+      <c r="J9" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
+      <c r="K9" s="28" t="s">
+        <v>72</v>
+      </c>
       <c r="L9" s="28"/>
       <c r="M9" s="28"/>
       <c r="N9" s="28"/>
-    </row>
-    <row r="10" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O9" s="28"/>
+    </row>
+    <row r="10" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="F10" s="4" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
+        <v>77</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
-    </row>
-    <row r="11" spans="1:14" ht="12.75">
+      <c r="O10" s="10"/>
+    </row>
+    <row r="11" spans="1:15" ht="12.75" customHeight="1">
       <c r="A11" s="21"/>
     </row>
-    <row r="12" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
+    <row r="12" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A12" s="27" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="J12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="I12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
-    </row>
-    <row r="13" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A13" s="11" t="s">
         <v>2</v>
       </c>
@@ -2107,81 +2144,87 @@
         <v>7</v>
       </c>
       <c r="D13" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="F13" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="G13" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="H13" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="29" t="s">
+      <c r="I13" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="29" t="s">
+      <c r="J13" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="28"/>
       <c r="K13" s="28"/>
       <c r="L13" s="28"/>
       <c r="M13" s="28"/>
       <c r="N13" s="28"/>
-    </row>
-    <row r="14" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O13" s="28"/>
+    </row>
+    <row r="14" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="G14" s="4" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J14" s="10"/>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
-    </row>
-    <row r="15" spans="1:14" ht="12.75">
+      <c r="O14" s="10"/>
+    </row>
+    <row r="15" spans="1:15" ht="12.75" customHeight="1">
       <c r="A15" s="21"/>
     </row>
-    <row r="16" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
+    <row r="16" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A16" s="27" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="J16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="I16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
-    </row>
-    <row r="17" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O16" s="5"/>
+    </row>
+    <row r="17" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A17" s="11" t="s">
         <v>2</v>
       </c>
@@ -2192,85 +2235,88 @@
         <v>7</v>
       </c>
       <c r="D17" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="F17" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="G17" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="29" t="s">
+      <c r="H17" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="29" t="s">
+      <c r="I17" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I17" s="29" t="s">
+      <c r="J17" s="29" t="s">
         <v>9</v>
-      </c>
-      <c r="J17" s="28" t="s">
-        <v>72</v>
       </c>
       <c r="K17" s="28"/>
       <c r="L17" s="28"/>
       <c r="M17" s="28"/>
       <c r="N17" s="28"/>
-    </row>
-    <row r="18" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O17" s="28"/>
+    </row>
+    <row r="18" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A18" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="H18" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
-    </row>
-    <row r="19" spans="1:14" ht="12.75">
+      <c r="O18" s="10"/>
+    </row>
+    <row r="19" spans="1:15" ht="12.75" customHeight="1">
       <c r="A19" s="21"/>
     </row>
-    <row r="20" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
+    <row r="20" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A20" s="27" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="B20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="J20" s="5"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="I20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
-    </row>
-    <row r="21" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A21" s="11" t="s">
         <v>2</v>
       </c>
@@ -2281,81 +2327,91 @@
         <v>7</v>
       </c>
       <c r="D21" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="F21" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="29" t="s">
+      <c r="G21" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="29" t="s">
+      <c r="H21" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="29" t="s">
+      <c r="I21" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I21" s="29" t="s">
+      <c r="J21" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
+      <c r="K21" s="28" t="s">
+        <v>72</v>
+      </c>
       <c r="L21" s="28"/>
       <c r="M21" s="28"/>
       <c r="N21" s="28"/>
-    </row>
-    <row r="22" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O21" s="28"/>
+    </row>
+    <row r="22" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="H22" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
+      <c r="K22" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
-    </row>
-    <row r="23" spans="1:14" ht="12.75">
+      <c r="O22" s="10"/>
+    </row>
+    <row r="23" spans="1:15" ht="12.75" customHeight="1">
       <c r="A23" s="21"/>
     </row>
-    <row r="24" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
+    <row r="24" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A24" s="27" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="B24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="J24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="I24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-    </row>
-    <row r="25" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A25" s="11" t="s">
         <v>2</v>
       </c>
@@ -2366,83 +2422,87 @@
         <v>7</v>
       </c>
       <c r="D25" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="F25" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="29" t="s">
+      <c r="G25" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G25" s="29" t="s">
+      <c r="H25" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H25" s="29" t="s">
+      <c r="I25" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I25" s="29" t="s">
+      <c r="J25" s="29" t="s">
         <v>9</v>
-      </c>
-      <c r="J25" s="28" t="s">
-        <v>29</v>
       </c>
       <c r="K25" s="28"/>
       <c r="L25" s="28"/>
       <c r="M25" s="28"/>
       <c r="N25" s="28"/>
-    </row>
-    <row r="26" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O25" s="28"/>
+    </row>
+    <row r="26" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A26" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="F26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="H26" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J26" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="J26" s="10" t="s">
-        <v>51</v>
       </c>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
-    </row>
-    <row r="27" spans="1:14" ht="12.75"/>
-    <row r="28" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O26" s="10"/>
+    </row>
+    <row r="27" spans="1:15" ht="12.75" customHeight="1">
+      <c r="A27" s="21"/>
+    </row>
+    <row r="28" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A28" s="27" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="B28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="J28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="I28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-    </row>
-    <row r="29" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A29" s="11" t="s">
         <v>2</v>
       </c>
@@ -2453,85 +2513,86 @@
         <v>7</v>
       </c>
       <c r="D29" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="29" t="s">
+      <c r="F29" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="29" t="s">
+      <c r="G29" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="29" t="s">
+      <c r="H29" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H29" s="29" t="s">
+      <c r="I29" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I29" s="29" t="s">
+      <c r="J29" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J29" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="K29" s="28"/>
+      <c r="K29" s="28" t="s">
+        <v>29</v>
+      </c>
       <c r="L29" s="28"/>
       <c r="M29" s="28"/>
       <c r="N29" s="28"/>
-    </row>
-    <row r="30" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O29" s="28"/>
+    </row>
+    <row r="30" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A30" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="29"/>
+      <c r="E30" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="F30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G30" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="H30" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J30" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K30" s="10"/>
+      <c r="K30" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
-    </row>
-    <row r="31" spans="1:14" ht="12.75">
-      <c r="A31" s="21"/>
-    </row>
-    <row r="32" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O30" s="10"/>
+    </row>
+    <row r="32" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A32" s="27" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="J32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="I32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
-    </row>
-    <row r="33" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O32" s="5"/>
+    </row>
+    <row r="33" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A33" s="11" t="s">
         <v>2</v>
       </c>
@@ -2542,81 +2603,89 @@
         <v>7</v>
       </c>
       <c r="D33" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="29" t="s">
+      <c r="F33" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F33" s="29" t="s">
+      <c r="G33" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G33" s="29" t="s">
+      <c r="H33" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="29" t="s">
+      <c r="I33" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I33" s="29" t="s">
+      <c r="J33" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
+      <c r="K33" s="28" t="s">
+        <v>57</v>
+      </c>
       <c r="L33" s="28"/>
       <c r="M33" s="28"/>
       <c r="N33" s="28"/>
-    </row>
-    <row r="34" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O33" s="28"/>
+    </row>
+    <row r="34" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A34" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="29"/>
+      <c r="E34" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="F34" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G34" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="H34" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
+      <c r="K34" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
-    </row>
-    <row r="35" spans="1:14" ht="12.75">
+      <c r="O34" s="10"/>
+    </row>
+    <row r="35" spans="1:15" ht="12.75" customHeight="1">
       <c r="A35" s="21"/>
     </row>
-    <row r="36" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
+    <row r="36" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A36" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="J36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="I36" s="5"/>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
-    </row>
-    <row r="37" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O36" s="5"/>
+    </row>
+    <row r="37" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A37" s="11" t="s">
         <v>2</v>
       </c>
@@ -2627,81 +2696,84 @@
         <v>7</v>
       </c>
       <c r="D37" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="29" t="s">
+      <c r="F37" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F37" s="29" t="s">
+      <c r="G37" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G37" s="29" t="s">
+      <c r="H37" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H37" s="29" t="s">
+      <c r="I37" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I37" s="29" t="s">
+      <c r="J37" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J37" s="28"/>
       <c r="K37" s="28"/>
       <c r="L37" s="28"/>
       <c r="M37" s="28"/>
       <c r="N37" s="28"/>
-    </row>
-    <row r="38" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O37" s="28"/>
+    </row>
+    <row r="38" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A38" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="E38" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E38" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="F38" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G38" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="H38" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J38" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J38" s="10"/>
       <c r="K38" s="10"/>
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
       <c r="N38" s="10"/>
-    </row>
-    <row r="39" spans="1:14" ht="12.75">
+      <c r="O38" s="10"/>
+    </row>
+    <row r="39" spans="1:15" ht="12.75" customHeight="1">
       <c r="A39" s="21"/>
     </row>
-    <row r="40" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
+    <row r="40" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A40" s="27" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="B40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="J40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="I40" s="5"/>
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
-    </row>
-    <row r="41" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O40" s="5"/>
+    </row>
+    <row r="41" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A41" s="11" t="s">
         <v>2</v>
       </c>
@@ -2712,79 +2784,84 @@
         <v>7</v>
       </c>
       <c r="D41" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E41" s="29" t="s">
+      <c r="F41" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F41" s="29" t="s">
+      <c r="G41" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G41" s="29" t="s">
+      <c r="H41" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H41" s="29" t="s">
+      <c r="I41" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I41" s="29" t="s">
+      <c r="J41" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J41" s="28"/>
       <c r="K41" s="28"/>
       <c r="L41" s="28"/>
       <c r="M41" s="28"/>
       <c r="N41" s="28"/>
-    </row>
-    <row r="42" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O41" s="28"/>
+    </row>
+    <row r="42" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A42" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="F42" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G42" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="H42" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I42" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J42" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J42" s="10"/>
       <c r="K42" s="10"/>
       <c r="L42" s="10"/>
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
-    </row>
-    <row r="43" spans="1:14" ht="12.75"/>
-    <row r="44" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O42" s="10"/>
+    </row>
+    <row r="43" spans="1:15" ht="12.75" customHeight="1">
+      <c r="A43" s="21"/>
+    </row>
+    <row r="44" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A44" s="27" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="B44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="J44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="I44" s="5"/>
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
-    </row>
-    <row r="45" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O44" s="5"/>
+    </row>
+    <row r="45" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A45" s="11" t="s">
         <v>2</v>
       </c>
@@ -2795,81 +2872,81 @@
         <v>7</v>
       </c>
       <c r="D45" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E45" s="29" t="s">
+      <c r="F45" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F45" s="29" t="s">
+      <c r="G45" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G45" s="29" t="s">
+      <c r="H45" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H45" s="29" t="s">
+      <c r="I45" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I45" s="29" t="s">
+      <c r="J45" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J45" s="28"/>
       <c r="K45" s="28"/>
       <c r="L45" s="28"/>
       <c r="M45" s="28"/>
       <c r="N45" s="28"/>
-    </row>
-    <row r="46" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O45" s="28"/>
+    </row>
+    <row r="46" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A46" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="F46" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F46" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="G46" s="4" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J46" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="K46" s="10"/>
       <c r="L46" s="10"/>
       <c r="M46" s="10"/>
       <c r="N46" s="10"/>
-    </row>
-    <row r="47" spans="1:14" ht="12.75">
-      <c r="A47" s="21"/>
-    </row>
-    <row r="48" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O46" s="10"/>
+    </row>
+    <row r="48" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A48" s="27" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="J48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="I48" s="5"/>
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
-    </row>
-    <row r="49" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O48" s="5"/>
+    </row>
+    <row r="49" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A49" s="11" t="s">
         <v>2</v>
       </c>
@@ -2880,85 +2957,84 @@
         <v>7</v>
       </c>
       <c r="D49" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E49" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E49" s="29" t="s">
+      <c r="F49" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F49" s="29" t="s">
+      <c r="G49" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G49" s="29" t="s">
+      <c r="H49" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H49" s="29" t="s">
+      <c r="I49" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I49" s="29" t="s">
+      <c r="J49" s="29" t="s">
         <v>9</v>
-      </c>
-      <c r="J49" s="28" t="s">
-        <v>29</v>
       </c>
       <c r="K49" s="28"/>
       <c r="L49" s="28"/>
       <c r="M49" s="28"/>
       <c r="N49" s="28"/>
-    </row>
-    <row r="50" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O49" s="28"/>
+    </row>
+    <row r="50" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A50" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="E50" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E50" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="F50" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G50" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G50" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="H50" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I50" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J50" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
       <c r="M50" s="10"/>
       <c r="N50" s="10"/>
-    </row>
-    <row r="51" spans="1:14" ht="12.75">
+      <c r="O50" s="10"/>
+    </row>
+    <row r="51" spans="1:15" ht="12.75" customHeight="1">
       <c r="A51" s="21"/>
     </row>
-    <row r="52" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
+    <row r="52" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A52" s="27" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="B52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="J52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="I52" s="5"/>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
-    </row>
-    <row r="53" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O52" s="5"/>
+    </row>
+    <row r="53" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A53" s="11" t="s">
         <v>2</v>
       </c>
@@ -2969,89 +3045,88 @@
         <v>7</v>
       </c>
       <c r="D53" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E53" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="29" t="s">
+      <c r="F53" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F53" s="29" t="s">
+      <c r="G53" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G53" s="29" t="s">
+      <c r="H53" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H53" s="29" t="s">
+      <c r="I53" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I53" s="29" t="s">
+      <c r="J53" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J53" s="28" t="s">
-        <v>57</v>
-      </c>
       <c r="K53" s="28" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="L53" s="28"/>
       <c r="M53" s="28"/>
       <c r="N53" s="28"/>
-    </row>
-    <row r="54" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O53" s="28"/>
+    </row>
+    <row r="54" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A54" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E54" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="F54" s="4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J54" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="K54" s="10" t="s">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="L54" s="10"/>
       <c r="M54" s="10"/>
       <c r="N54" s="10"/>
-    </row>
-    <row r="55" spans="1:14" ht="12.75">
+      <c r="O54" s="10"/>
+    </row>
+    <row r="55" spans="1:15" ht="12.75" customHeight="1">
       <c r="A55" s="21"/>
     </row>
-    <row r="56" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
+    <row r="56" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A56" s="27" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="H56" s="5"/>
-      <c r="J56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="I56" s="5"/>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
       <c r="M56" s="5"/>
       <c r="N56" s="5"/>
-    </row>
-    <row r="57" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O56" s="5"/>
+    </row>
+    <row r="57" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A57" s="11" t="s">
         <v>2</v>
       </c>
@@ -3062,89 +3137,92 @@
         <v>7</v>
       </c>
       <c r="D57" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E57" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="29" t="s">
+      <c r="F57" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F57" s="29" t="s">
+      <c r="G57" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G57" s="29" t="s">
+      <c r="H57" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H57" s="29" t="s">
+      <c r="I57" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I57" s="29" t="s">
+      <c r="J57" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J57" s="28" t="s">
+      <c r="K57" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="K57" s="28" t="s">
+      <c r="L57" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="L57" s="28"/>
       <c r="M57" s="28"/>
       <c r="N57" s="28"/>
-    </row>
-    <row r="58" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O57" s="28"/>
+    </row>
+    <row r="58" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A58" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="E58" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="F58" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F58" s="4" t="s">
+      <c r="G58" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G58" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="H58" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I58" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J58" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J58" s="10" t="s">
-        <v>67</v>
-      </c>
       <c r="K58" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="L58" s="10"/>
+        <v>66</v>
+      </c>
+      <c r="L58" s="10" t="s">
+        <v>3</v>
+      </c>
       <c r="M58" s="10"/>
       <c r="N58" s="10"/>
-    </row>
-    <row r="59" spans="1:14" ht="12.75">
+      <c r="O58" s="10"/>
+    </row>
+    <row r="59" spans="1:15" ht="12.75" customHeight="1">
       <c r="A59" s="21"/>
     </row>
-    <row r="60" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
+    <row r="60" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A60" s="27" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="J60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="I60" s="5"/>
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
       <c r="M60" s="5"/>
       <c r="N60" s="5"/>
-    </row>
-    <row r="61" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O60" s="5"/>
+    </row>
+    <row r="61" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A61" s="11" t="s">
         <v>2</v>
       </c>
@@ -3155,81 +3233,92 @@
         <v>7</v>
       </c>
       <c r="D61" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E61" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E61" s="29" t="s">
+      <c r="F61" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F61" s="29" t="s">
+      <c r="G61" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G61" s="29" t="s">
+      <c r="H61" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H61" s="29" t="s">
+      <c r="I61" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I61" s="29" t="s">
+      <c r="J61" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J61" s="28"/>
-      <c r="K61" s="28"/>
-      <c r="L61" s="28"/>
+      <c r="K61" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="L61" s="28" t="s">
+        <v>59</v>
+      </c>
       <c r="M61" s="28"/>
       <c r="N61" s="28"/>
-    </row>
-    <row r="62" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O61" s="28"/>
+    </row>
+    <row r="62" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A62" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D62" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="F62" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F62" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="G62" s="4" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="H62" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J62" s="10"/>
-      <c r="K62" s="10"/>
-      <c r="L62" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K62" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="L62" s="10" t="s">
+        <v>3</v>
+      </c>
       <c r="M62" s="10"/>
       <c r="N62" s="10"/>
-    </row>
-    <row r="63" spans="1:14" ht="12.75">
+      <c r="O62" s="10"/>
+    </row>
+    <row r="63" spans="1:15" ht="12.75" customHeight="1">
       <c r="A63" s="21"/>
     </row>
-    <row r="64" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
+    <row r="64" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A64" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="H64" s="5"/>
-      <c r="J64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="I64" s="5"/>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
       <c r="M64" s="5"/>
       <c r="N64" s="5"/>
-    </row>
-    <row r="65" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O64" s="5"/>
+    </row>
+    <row r="65" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A65" s="11" t="s">
         <v>2</v>
       </c>
@@ -3240,85 +3329,84 @@
         <v>7</v>
       </c>
       <c r="D65" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E65" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E65" s="29" t="s">
+      <c r="F65" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F65" s="29" t="s">
+      <c r="G65" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G65" s="29" t="s">
+      <c r="H65" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H65" s="29" t="s">
+      <c r="I65" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I65" s="29" t="s">
+      <c r="J65" s="29" t="s">
         <v>9</v>
-      </c>
-      <c r="J65" s="28" t="s">
-        <v>29</v>
       </c>
       <c r="K65" s="28"/>
       <c r="L65" s="28"/>
       <c r="M65" s="28"/>
       <c r="N65" s="28"/>
-    </row>
-    <row r="66" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O65" s="28"/>
+    </row>
+    <row r="66" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A66" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="E66" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E66" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="F66" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G66" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G66" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="H66" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I66" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J66" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="J66" s="10" t="s">
-        <v>30</v>
       </c>
       <c r="K66" s="10"/>
       <c r="L66" s="10"/>
       <c r="M66" s="10"/>
       <c r="N66" s="10"/>
-    </row>
-    <row r="67" spans="1:14" ht="12.75">
+      <c r="O66" s="10"/>
+    </row>
+    <row r="67" spans="1:15" ht="12.75" customHeight="1">
       <c r="A67" s="21"/>
     </row>
-    <row r="68" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
+    <row r="68" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A68" s="27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="J68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="I68" s="5"/>
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
       <c r="M68" s="5"/>
       <c r="N68" s="5"/>
-    </row>
-    <row r="69" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O68" s="5"/>
+    </row>
+    <row r="69" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A69" s="11" t="s">
         <v>2</v>
       </c>
@@ -3329,81 +3417,88 @@
         <v>7</v>
       </c>
       <c r="D69" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E69" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E69" s="29" t="s">
+      <c r="F69" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F69" s="29" t="s">
+      <c r="G69" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G69" s="29" t="s">
+      <c r="H69" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H69" s="29" t="s">
+      <c r="I69" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I69" s="29" t="s">
+      <c r="J69" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J69" s="28"/>
-      <c r="K69" s="28"/>
+      <c r="K69" s="28" t="s">
+        <v>29</v>
+      </c>
       <c r="L69" s="28"/>
       <c r="M69" s="28"/>
       <c r="N69" s="28"/>
-    </row>
-    <row r="70" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O69" s="28"/>
+    </row>
+    <row r="70" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A70" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="E70" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E70" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="F70" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="H70" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I70" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J70" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J70" s="10"/>
-      <c r="K70" s="10"/>
+      <c r="K70" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="L70" s="10"/>
       <c r="M70" s="10"/>
       <c r="N70" s="10"/>
-    </row>
-    <row r="71" spans="1:14" ht="12.75">
+      <c r="O70" s="10"/>
+    </row>
+    <row r="71" spans="1:15" ht="12.75" customHeight="1">
       <c r="A71" s="21"/>
     </row>
-    <row r="72" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1">
+    <row r="72" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A72" s="27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="F72" s="5"/>
-      <c r="H72" s="5"/>
-      <c r="J72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="I72" s="5"/>
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
       <c r="M72" s="5"/>
       <c r="N72" s="5"/>
-    </row>
-    <row r="73" spans="1:14" s="7" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O72" s="5"/>
+    </row>
+    <row r="73" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A73" s="11" t="s">
         <v>2</v>
       </c>
@@ -3414,85 +3509,87 @@
         <v>7</v>
       </c>
       <c r="D73" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E73" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E73" s="29" t="s">
+      <c r="F73" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F73" s="29" t="s">
+      <c r="G73" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G73" s="29" t="s">
+      <c r="H73" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H73" s="29" t="s">
+      <c r="I73" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I73" s="29" t="s">
+      <c r="J73" s="29" t="s">
         <v>9</v>
-      </c>
-      <c r="J73" s="28" t="s">
-        <v>29</v>
       </c>
       <c r="K73" s="28"/>
       <c r="L73" s="28"/>
       <c r="M73" s="28"/>
       <c r="N73" s="28"/>
-    </row>
-    <row r="74" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O73" s="28"/>
+    </row>
+    <row r="74" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A74" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D74" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E74" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E74" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="F74" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G74" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G74" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="H74" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I74" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J74" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="J74" s="10" t="s">
-        <v>30</v>
       </c>
       <c r="K74" s="10"/>
       <c r="L74" s="10"/>
       <c r="M74" s="10"/>
       <c r="N74" s="10"/>
-    </row>
-    <row r="75" spans="1:14" ht="12.75">
+      <c r="O74" s="10"/>
+    </row>
+    <row r="75" spans="1:15" ht="12.75" customHeight="1">
       <c r="A75" s="21"/>
     </row>
-    <row r="76" spans="1:14" s="6" customFormat="1" ht="25.5">
+    <row r="76" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
       <c r="A76" s="27" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="B76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="H76" s="5"/>
-      <c r="J76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="I76" s="5"/>
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
       <c r="M76" s="5"/>
       <c r="N76" s="5"/>
-    </row>
-    <row r="77" spans="1:14" s="7" customFormat="1" ht="38.25">
+      <c r="O76" s="5"/>
+    </row>
+    <row r="77" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A77" s="11" t="s">
         <v>2</v>
       </c>
@@ -3503,62 +3600,157 @@
         <v>7</v>
       </c>
       <c r="D77" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E77" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E77" s="29" t="s">
+      <c r="F77" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F77" s="29" t="s">
+      <c r="G77" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G77" s="29" t="s">
+      <c r="H77" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H77" s="29" t="s">
+      <c r="I77" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I77" s="29" t="s">
+      <c r="J77" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J77" s="28"/>
-      <c r="K77" s="28"/>
+      <c r="K77" s="28" t="s">
+        <v>29</v>
+      </c>
       <c r="L77" s="28"/>
       <c r="M77" s="28"/>
       <c r="N77" s="28"/>
-    </row>
-    <row r="78" spans="1:14" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="O77" s="28"/>
+    </row>
+    <row r="78" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A78" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D78" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E78" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E78" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="F78" s="4" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="H78" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J78" s="10"/>
-      <c r="K78" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="J78" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K78" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="L78" s="10"/>
       <c r="M78" s="10"/>
       <c r="N78" s="10"/>
+      <c r="O78" s="10"/>
+    </row>
+    <row r="79" spans="1:15" ht="12.75" customHeight="1">
+      <c r="A79" s="21"/>
+    </row>
+    <row r="80" spans="1:15" s="6" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A80" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="I80" s="5"/>
+      <c r="K80" s="5"/>
+      <c r="L80" s="5"/>
+      <c r="M80" s="5"/>
+      <c r="N80" s="5"/>
+      <c r="O80" s="5"/>
+    </row>
+    <row r="81" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A81" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E81" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F81" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H81" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="I81" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="J81" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K81" s="28"/>
+      <c r="L81" s="28"/>
+      <c r="M81" s="28"/>
+      <c r="N81" s="28"/>
+      <c r="O81" s="28"/>
+    </row>
+    <row r="82" spans="1:15" s="4" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A82" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I82" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J82" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K82" s="10"/>
+      <c r="L82" s="10"/>
+      <c r="M82" s="10"/>
+      <c r="N82" s="10"/>
+      <c r="O82" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>